<commit_message>
Linked Item Database with Inventory
- The item database is linked with the inventory system, allowing for pulling items and reading them in the inventory
</commit_message>
<xml_diff>
--- a/datafiles/item_data.xlsx
+++ b/datafiles/item_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>health_potion_light</t>
   </si>
@@ -59,6 +59,15 @@
   </si>
   <si>
     <t>armor_potion_critical</t>
+  </si>
+  <si>
+    <t>spr_health_potion_light</t>
+  </si>
+  <si>
+    <t>spr_armor_potion_light</t>
+  </si>
+  <si>
+    <t>spr_placeholder</t>
   </si>
 </sst>
 </file>
@@ -430,7 +439,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,8 +481,8 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
-        <v>-1</v>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -499,8 +508,8 @@
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2">
-        <v>-1</v>
+      <c r="B3" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
@@ -526,8 +535,8 @@
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="2">
-        <v>-1</v>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
@@ -553,8 +562,8 @@
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2">
-        <v>-1</v>
+      <c r="B5" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C5" s="2">
         <v>4</v>
@@ -580,8 +589,8 @@
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="2">
-        <v>-1</v>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -607,8 +616,8 @@
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2">
-        <v>-1</v>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C7" s="2">
         <v>2</v>
@@ -634,8 +643,8 @@
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2">
-        <v>-1</v>
+      <c r="B8" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C8" s="2">
         <v>3</v>
@@ -661,8 +670,8 @@
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="2">
-        <v>-1</v>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C9" s="2">
         <v>4</v>

</xml_diff>

<commit_message>
Added Item Use Menu
- Added pop-up when right clicking items. This shows the name of the item, the description for the item, and a button to use.

- Added use button

- Updated item data structs and files with new data

- Fixed item remove script
</commit_message>
<xml_diff>
--- a/datafiles/item_data.xlsx
+++ b/datafiles/item_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>health_potion_light</t>
   </si>
@@ -74,6 +74,63 @@
   </si>
   <si>
     <t>spr_armor_potion_moderate</t>
+  </si>
+  <si>
+    <t>scr</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Light Health Potion</t>
+  </si>
+  <si>
+    <t>Moderate Health Potion</t>
+  </si>
+  <si>
+    <t>Severe Health Potion</t>
+  </si>
+  <si>
+    <t>Critical Health Potion</t>
+  </si>
+  <si>
+    <t>Light Armor Potion</t>
+  </si>
+  <si>
+    <t>Moderate Armor Potion</t>
+  </si>
+  <si>
+    <t>Severe Armor Potion</t>
+  </si>
+  <si>
+    <t>Critical Armor Potion</t>
+  </si>
+  <si>
+    <t>Heal 1d8 + 1</t>
+  </si>
+  <si>
+    <t>Heal 2d8 + 3</t>
+  </si>
+  <si>
+    <t>Heal 3d8 + 5</t>
+  </si>
+  <si>
+    <t>Heal 4d8 + 7</t>
+  </si>
+  <si>
+    <t>Repair 1d8 + 1 Armor</t>
+  </si>
+  <si>
+    <t>Repair 2d8 + 3 Armor</t>
+  </si>
+  <si>
+    <t>Repair 3d8 + 5 Armor</t>
+  </si>
+  <si>
+    <t>Repair 4d8 + 7 Armor</t>
   </si>
 </sst>
 </file>
@@ -124,19 +181,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -442,361 +496,436 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" customWidth="1"/>
     <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+    <col min="10" max="10" width="22.5703125" customWidth="1"/>
+    <col min="11" max="11" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="J1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D2" s="2">
         <v>1</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>8</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>1</v>
       </c>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
       <c r="G2" s="2">
         <v>0</v>
       </c>
       <c r="H2" s="2">
         <v>0</v>
       </c>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="I2" s="2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D3" s="2">
         <v>2</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>8</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>3</v>
       </c>
-      <c r="F3" s="2">
-        <v>0</v>
-      </c>
       <c r="G3" s="2">
         <v>0</v>
       </c>
       <c r="H3" s="2">
         <v>0</v>
       </c>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="I3" s="2">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D4" s="2">
         <v>3</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>8</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>5</v>
       </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
       <c r="G4" s="2">
         <v>0</v>
       </c>
       <c r="H4" s="2">
         <v>0</v>
       </c>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D5" s="2">
         <v>4</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="2">
         <v>8</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <v>7</v>
       </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
       <c r="G5" s="2">
         <v>0</v>
       </c>
       <c r="H5" s="2">
         <v>0</v>
       </c>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D6" s="2">
         <v>1</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="2">
         <v>8</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <v>1</v>
       </c>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
       <c r="G6" s="2">
         <v>0</v>
       </c>
       <c r="H6" s="2">
         <v>0</v>
       </c>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="I6" s="2">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D7" s="2">
         <v>2</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7" s="2">
         <v>8</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="2">
         <v>3</v>
       </c>
-      <c r="F7" s="2">
-        <v>0</v>
-      </c>
       <c r="G7" s="2">
         <v>0</v>
       </c>
       <c r="H7" s="2">
         <v>0</v>
       </c>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="I7" s="2">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D8" s="2">
         <v>3</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E8" s="2">
         <v>8</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="2">
         <v>5</v>
       </c>
-      <c r="F8" s="2">
-        <v>0</v>
-      </c>
       <c r="G8" s="2">
         <v>0</v>
       </c>
       <c r="H8" s="2">
         <v>0</v>
       </c>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="I8" s="2">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D9" s="2">
         <v>4</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E9" s="2">
         <v>8</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" s="2">
         <v>7</v>
       </c>
-      <c r="F9" s="2">
-        <v>0</v>
-      </c>
       <c r="G9" s="2">
         <v>0</v>
       </c>
       <c r="H9" s="2">
         <v>0</v>
       </c>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
+      <c r="I9" s="2">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Severe and Critical Potions
- See title.
</commit_message>
<xml_diff>
--- a/datafiles/item_data.xlsx
+++ b/datafiles/item_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>health_potion_light</t>
   </si>
@@ -67,9 +67,6 @@
     <t>spr_armor_potion_light</t>
   </si>
   <si>
-    <t>spr_placeholder</t>
-  </si>
-  <si>
     <t>spr_health_potion_moderate</t>
   </si>
   <si>
@@ -131,6 +128,18 @@
   </si>
   <si>
     <t>Repair 4d8 + 7 Armor</t>
+  </si>
+  <si>
+    <t>spr_armor_potion_severe</t>
+  </si>
+  <si>
+    <t>spr_health_potion_severe</t>
+  </si>
+  <si>
+    <t>spr_health_potion_critical</t>
+  </si>
+  <si>
+    <t>spr_armor_potion_critical</t>
   </si>
 </sst>
 </file>
@@ -499,7 +508,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,7 +530,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -542,10 +551,10 @@
         <v>7</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -577,10 +586,10 @@
         <v>0</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -588,7 +597,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="2">
         <v>-1</v>
@@ -612,10 +621,10 @@
         <v>0</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -623,7 +632,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="C4" s="2">
         <v>-1</v>
@@ -647,10 +656,10 @@
         <v>0</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -658,7 +667,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="C5" s="2">
         <v>-1</v>
@@ -682,10 +691,10 @@
         <v>0</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -717,10 +726,10 @@
         <v>0</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -728,7 +737,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="2">
         <v>-1</v>
@@ -752,10 +761,10 @@
         <v>0</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -763,7 +772,7 @@
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="C8" s="2">
         <v>-1</v>
@@ -787,10 +796,10 @@
         <v>0</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -798,7 +807,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="C9" s="2">
         <v>-1</v>
@@ -822,10 +831,10 @@
         <v>0</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added Armor Potion Functionality
- Armor potions now regen armor based on CSV data, then instantly begin passive armor regeneration
</commit_message>
<xml_diff>
--- a/datafiles/item_data.xlsx
+++ b/datafiles/item_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
   <si>
     <t>health_potion_light</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>scr_health_potion</t>
+  </si>
+  <si>
+    <t>scr_armor_potion</t>
   </si>
 </sst>
 </file>
@@ -511,7 +514,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,8 +710,8 @@
       <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="2">
-        <v>-1</v>
+      <c r="C6" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
@@ -742,8 +745,8 @@
       <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="2">
-        <v>-1</v>
+      <c r="C7" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="D7" s="2">
         <v>2</v>
@@ -777,8 +780,8 @@
       <c r="B8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="2">
-        <v>-1</v>
+      <c r="C8" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="D8" s="2">
         <v>3</v>
@@ -812,8 +815,8 @@
       <c r="B9" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="2">
-        <v>-1</v>
+      <c r="C9" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="D9" s="2">
         <v>4</v>

</xml_diff>